<commit_message>
Update BTaDLP and BFCpUEbS for more recent EIA data
</commit_message>
<xml_diff>
--- a/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
+++ b/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BTaDLP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\BTaDLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Calculations" sheetId="4" r:id="rId3"/>
     <sheet name="BTaDLP" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="35">
   <si>
     <t>Source:</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>BTaDLP BAU Transmission and Distribution Loss Percentage</t>
-  </si>
-  <si>
-    <t>http://www.eia.gov/totalenergy/data/monthly/#electricity</t>
   </si>
   <si>
     <t>U.S. Energy Information Administration</t>
@@ -90,9 +87,6 @@
     <t>Net Generation: Electric Power Sector</t>
   </si>
   <si>
-    <t>Billion Kilowatthours</t>
-  </si>
-  <si>
     <t>Next Update: October 26, 2016</t>
   </si>
   <si>
@@ -124,6 +118,15 @@
   </si>
   <si>
     <t>Trans and Dist Loss Perc (dimensionless)</t>
+  </si>
+  <si>
+    <t>(Billion Kilowatthours)</t>
+  </si>
+  <si>
+    <t>June 2020 Monthly Energy Review</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/totalenergy/data/monthly/</t>
   </si>
 </sst>
 </file>
@@ -222,7 +225,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -232,10 +235,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -244,6 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -291,10 +291,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Calculations!$D$2:$D$17</c:f>
+              <c:f>Calculations!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>6.6944071098814603E-2</c:v>
                 </c:pt>
@@ -341,7 +341,19 @@
                   <c:v>6.18602525829927E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.3923968962333539E-2</c:v>
+                  <c:v>6.2284686986993069E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.1476826137713443E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.8315084670271959E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.456342836151426E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.6105782903553054E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -736,17 +748,17 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,44 +766,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" location="electricity"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -800,2664 +812,2819 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:XFD64"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="9" style="6"/>
+    <col min="1" max="1" width="9" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="str">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="str">
         <f>HYPERLINK("http://www.eia.gov/totalenergy/data/monthly/dataunits.cfm","Note: Information about data precision.")</f>
         <v>Note: Information about data precision.</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="H11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="I11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="K11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="L11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
         <v>1949</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13">
         <v>291.10000000000002</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
         <v>5.0250000000000004</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13">
         <v>296.12400000000002</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13">
         <v>1.764</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13">
         <v>0.17499999999999999</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13">
         <v>1.5880000000000001</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13">
         <v>43.201000000000001</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13">
         <v>254.511</v>
       </c>
-      <c r="K13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="6">
+      <c r="K13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13">
         <v>254.511</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="2">
         <v>1950</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14">
         <v>329.14100000000002</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
         <v>4.9459999999999997</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14">
         <v>334.08800000000002</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14">
         <v>1.9330000000000001</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14">
         <v>0.14699999999999999</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14">
         <v>1.786</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14">
         <v>44.43</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14">
         <v>291.44299999999998</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="6">
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14">
         <v>291.44299999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="2">
         <v>1951</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15">
         <v>370.673</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
         <v>4.6260000000000003</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15">
         <v>375.298</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15">
         <v>2.387</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15">
         <v>0.2</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15">
         <v>2.1869999999999998</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15">
         <v>47.201000000000001</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15">
         <v>330.28500000000003</v>
       </c>
-      <c r="K15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="6">
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15">
         <v>330.28500000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="2">
         <v>1952</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16">
         <v>399.22399999999999</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="6">
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
         <v>4.6059999999999999</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16">
         <v>403.82900000000001</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16">
         <v>2.5059999999999998</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16">
         <v>0.23699999999999999</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16">
         <v>2.2690000000000001</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16">
         <v>49.933999999999997</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16">
         <v>356.16399999999999</v>
       </c>
-      <c r="K16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="6">
+      <c r="K16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16">
         <v>356.16399999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="2">
         <v>1953</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17">
         <v>442.66500000000002</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17">
         <v>4.3840000000000003</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17">
         <v>447.04899999999998</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17">
         <v>2.4369999999999998</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17">
         <v>0.42899999999999999</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17">
         <v>2.008</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17">
         <v>52.84</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17">
         <v>396.21699999999998</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="6">
+      <c r="K17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17">
         <v>396.21699999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="2">
         <v>1954</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18">
         <v>471.68599999999998</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="6">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18">
         <v>4.5709999999999997</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18">
         <v>476.25799999999998</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18">
         <v>2.6880000000000002</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18">
         <v>0.34799999999999998</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18">
         <v>2.34</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18">
         <v>54.433999999999997</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18">
         <v>424.16399999999999</v>
       </c>
-      <c r="K18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="6">
+      <c r="K18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18">
         <v>424.16399999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="2">
         <v>1955</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19">
         <v>547.03800000000001</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="6">
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19">
         <v>3.2610000000000001</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19">
         <v>550.29899999999998</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19">
         <v>4.5670000000000002</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19">
         <v>0.5</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19">
         <v>4.0679999999999996</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19">
         <v>57.618000000000002</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19">
         <v>496.74799999999999</v>
       </c>
-      <c r="K19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="6">
+      <c r="K19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19">
         <v>496.74799999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="2">
         <v>1956</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20">
         <v>600.66800000000001</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="6">
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
         <v>3.2080000000000002</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20">
         <v>603.87599999999998</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20">
         <v>5.1790000000000003</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20">
         <v>0.63100000000000001</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20">
         <v>4.548</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20">
         <v>62.143999999999998</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20">
         <v>546.28</v>
       </c>
-      <c r="K20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="6">
+      <c r="K20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20">
         <v>546.28</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="2">
         <v>1957</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21">
         <v>631.51700000000005</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="6">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
         <v>3.125</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21">
         <v>634.64200000000005</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21">
         <v>4.8559999999999999</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21">
         <v>1.254</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21">
         <v>3.601</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21">
         <v>62.423999999999999</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21">
         <v>575.82000000000005</v>
       </c>
-      <c r="K21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="6">
+      <c r="K21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21">
         <v>575.82000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="2">
         <v>1958</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22">
         <v>645.09799999999996</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="6">
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22">
         <v>3.3519999999999999</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22">
         <v>648.45100000000002</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22">
         <v>4.0780000000000003</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22">
         <v>0.76</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22">
         <v>3.3180000000000001</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22">
         <v>63.905999999999999</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22">
         <v>587.86300000000006</v>
       </c>
-      <c r="K22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="6">
+      <c r="K22" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22">
         <v>587.86300000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="2">
         <v>1959</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23">
         <v>710.00599999999997</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="6">
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23">
         <v>3.3730000000000002</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23">
         <v>713.37900000000002</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23">
         <v>4.3929999999999998</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23">
         <v>0.83799999999999997</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23">
         <v>3.5539999999999998</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23">
         <v>70.045000000000002</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23">
         <v>646.88800000000003</v>
       </c>
-      <c r="K23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="6">
+      <c r="K23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23">
         <v>646.88800000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="2">
         <v>1960</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24">
         <v>755.54899999999998</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="6">
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24">
         <v>3.6070000000000002</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24">
         <v>759.15599999999995</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24">
         <v>5.3230000000000004</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24">
         <v>0.78800000000000003</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24">
         <v>4.5350000000000001</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24">
         <v>75.616</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24">
         <v>688.07500000000005</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="6">
+      <c r="K24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24">
         <v>688.07500000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="2">
         <v>1961</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25">
         <v>793.76</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="6">
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25">
         <v>3.3650000000000002</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25">
         <v>797.12400000000002</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25">
         <v>3.17</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25">
         <v>0.91700000000000004</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25">
         <v>2.254</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25">
         <v>77.427999999999997</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25">
         <v>721.95</v>
       </c>
-      <c r="K25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="6">
+      <c r="K25" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25">
         <v>721.95</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A26" s="2">
         <v>1962</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26">
         <v>854.53499999999997</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="6">
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26">
         <v>3.4089999999999998</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26">
         <v>857.94399999999996</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26">
         <v>2.1970000000000001</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26">
         <v>1.661</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26">
         <v>0.53600000000000003</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26">
         <v>80.88</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26">
         <v>777.6</v>
       </c>
-      <c r="K26" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="6">
+      <c r="K26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26">
         <v>777.6</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
         <v>1963</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27">
         <v>916.79300000000001</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="6">
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27">
         <v>3.2349999999999999</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27">
         <v>920.02800000000002</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27">
         <v>2.0830000000000002</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27">
         <v>1.9850000000000001</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27">
         <v>87.513000000000005</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27">
         <v>832.61300000000006</v>
       </c>
-      <c r="K27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" s="6">
+      <c r="K27" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27">
         <v>832.61300000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A28" s="2">
         <v>1964</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28">
         <v>983.99</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="6">
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28">
         <v>3.2280000000000002</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28">
         <v>987.21799999999996</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28">
         <v>6.2089999999999996</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28">
         <v>4.2530000000000001</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28">
         <v>1.9550000000000001</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28">
         <v>93.114999999999995</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J28">
         <v>896.05899999999997</v>
       </c>
-      <c r="K28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="6">
+      <c r="K28" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28">
         <v>896.05899999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A29" s="2">
         <v>1965</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29">
         <v>1055.252</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="6">
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29">
         <v>3.1339999999999999</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29">
         <v>1058.386</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29">
         <v>3.5579999999999998</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29">
         <v>3.6989999999999998</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29">
         <v>-0.14099999999999999</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29">
         <v>104.455</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29">
         <v>953.78899999999999</v>
       </c>
-      <c r="K29" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L29" s="6">
+      <c r="K29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29">
         <v>953.78899999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" s="2">
         <v>1966</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30">
         <v>1144.3499999999999</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="6">
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30">
         <v>3.1819999999999999</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30">
         <v>1147.5319999999999</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30">
         <v>4.2679999999999998</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30">
         <v>3.1760000000000002</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30">
         <v>1.0920000000000001</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30">
         <v>113.479</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30">
         <v>1035.145</v>
       </c>
-      <c r="K30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" s="6">
+      <c r="K30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30">
         <v>1035.145</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" s="2">
         <v>1967</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31">
         <v>1214.365</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="6">
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31">
         <v>3.431</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31">
         <v>1217.796</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31">
         <v>4.0510000000000002</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31">
         <v>4.3499999999999996</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31">
         <v>-0.29899999999999999</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31">
         <v>118.279</v>
       </c>
-      <c r="J31" s="6">
+      <c r="J31">
         <v>1099.2170000000001</v>
       </c>
-      <c r="K31" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L31" s="6">
+      <c r="K31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31">
         <v>1099.2170000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A32" s="2">
         <v>1968</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32">
         <v>1329.443</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="6">
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32">
         <v>3.383</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32">
         <v>1332.826</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32">
         <v>3.6539999999999999</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32">
         <v>4.2850000000000001</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32">
         <v>-0.63100000000000001</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32">
         <v>129.32400000000001</v>
       </c>
-      <c r="J32" s="6">
+      <c r="J32">
         <v>1202.8710000000001</v>
       </c>
-      <c r="K32" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="6">
+      <c r="K32" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32">
         <v>1202.8710000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A33" s="2">
         <v>1969</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33">
         <v>1442.182</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="6">
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33">
         <v>3.2759999999999998</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33">
         <v>1445.4580000000001</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33">
         <v>4.9020000000000001</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33">
         <v>3.83</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H33">
         <v>1.0720000000000001</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33">
         <v>132.696</v>
       </c>
-      <c r="J33" s="6">
+      <c r="J33">
         <v>1313.8330000000001</v>
       </c>
-      <c r="K33" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L33" s="6">
+      <c r="K33" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33">
         <v>1313.8330000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A34" s="2">
         <v>1970</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34">
         <v>1531.8679999999999</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="6">
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34">
         <v>3.2440000000000002</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34">
         <v>1535.1110000000001</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34">
         <v>6.17</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34">
         <v>4.2089999999999996</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34">
         <v>1.96</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34">
         <v>144.77199999999999</v>
       </c>
-      <c r="J34" s="6">
+      <c r="J34">
         <v>1392.3</v>
       </c>
-      <c r="K34" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L34" s="6">
+      <c r="K34" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34">
         <v>1392.3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A35" s="2">
         <v>1971</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35">
         <v>1612.633</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="6">
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35">
         <v>3.2210000000000001</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35">
         <v>1615.854</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35">
         <v>7.0439999999999996</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35">
         <v>3.5139999999999998</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35">
         <v>3.53</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35">
         <v>149.84399999999999</v>
       </c>
-      <c r="J35" s="6">
+      <c r="J35">
         <v>1469.54</v>
       </c>
-      <c r="K35" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="6">
+      <c r="K35" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35">
         <v>1469.54</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A36" s="2">
         <v>1972</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36">
         <v>1749.662</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="6">
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36">
         <v>3.3159999999999998</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36">
         <v>1752.9780000000001</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36">
         <v>10.494999999999999</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36">
         <v>2.8090000000000002</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H36">
         <v>7.6870000000000003</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36">
         <v>165.50399999999999</v>
       </c>
-      <c r="J36" s="6">
+      <c r="J36">
         <v>1595.1610000000001</v>
       </c>
-      <c r="K36" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="6">
+      <c r="K36" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36">
         <v>1595.1610000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A37" s="2">
         <v>1973</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37">
         <v>1860.71</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="6">
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37">
         <v>3.347</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37">
         <v>1864.057</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37">
         <v>16.847999999999999</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37">
         <v>2.57</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37">
         <v>14.278</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37">
         <v>165.42599999999999</v>
       </c>
-      <c r="J37" s="6">
+      <c r="J37">
         <v>1712.9090000000001</v>
       </c>
-      <c r="K37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="6">
+      <c r="K37" t="s">
+        <v>19</v>
+      </c>
+      <c r="L37">
         <v>1712.9090000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A38" s="2">
         <v>1974</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38">
         <v>1867.14</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="6">
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38">
         <v>3.18</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38">
         <v>1870.319</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38">
         <v>15.42</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38">
         <v>2.726</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38">
         <v>12.694000000000001</v>
       </c>
-      <c r="I38" s="6">
+      <c r="I38">
         <v>177.089</v>
       </c>
-      <c r="J38" s="6">
+      <c r="J38">
         <v>1705.924</v>
       </c>
-      <c r="K38" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="6">
+      <c r="K38" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38">
         <v>1705.924</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A39" s="2">
         <v>1975</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39">
         <v>1917.6489999999999</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="6">
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39">
         <v>3.1059999999999999</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39">
         <v>1920.7550000000001</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39">
         <v>11.268000000000001</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39">
         <v>5.0830000000000002</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39">
         <v>6.1849999999999996</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39">
         <v>179.84899999999999</v>
       </c>
-      <c r="J39" s="6">
+      <c r="J39">
         <v>1747.0909999999999</v>
       </c>
-      <c r="K39" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="6">
+      <c r="K39" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39">
         <v>1747.0909999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A40" s="2">
         <v>1976</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40">
         <v>2037.6959999999999</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="6">
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40">
         <v>3.2170000000000001</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40">
         <v>2040.914</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40">
         <v>10.988</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40">
         <v>2.3780000000000001</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40">
         <v>8.61</v>
       </c>
-      <c r="I40" s="6">
+      <c r="I40">
         <v>194.27799999999999</v>
       </c>
-      <c r="J40" s="6">
+      <c r="J40">
         <v>1855.2460000000001</v>
       </c>
-      <c r="K40" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="6">
+      <c r="K40" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40">
         <v>1855.2460000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A41" s="2">
         <v>1977</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41">
         <v>2124.3229999999999</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="6">
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41">
         <v>3.1240000000000001</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41">
         <v>2127.4470000000001</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41">
         <v>20.158999999999999</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41">
         <v>2.7440000000000002</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41">
         <v>17.416</v>
       </c>
-      <c r="I41" s="6">
+      <c r="I41">
         <v>196.50200000000001</v>
       </c>
-      <c r="J41" s="6">
+      <c r="J41">
         <v>1948.3610000000001</v>
       </c>
-      <c r="K41" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="6">
+      <c r="K41" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41">
         <v>1948.3610000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A42" s="2">
         <v>1978</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42">
         <v>2206.3310000000001</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="6">
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42">
         <v>3.0459999999999998</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42">
         <v>2209.377</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42">
         <v>21.207999999999998</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42">
         <v>1.478</v>
       </c>
-      <c r="H42" s="6">
+      <c r="H42">
         <v>19.73</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I42">
         <v>211.185</v>
       </c>
-      <c r="J42" s="6">
+      <c r="J42">
         <v>2017.922</v>
       </c>
-      <c r="K42" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="6">
+      <c r="K42" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42">
         <v>2017.922</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A43" s="2">
         <v>1979</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43">
         <v>2247.3719999999998</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="6">
+      <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43">
         <v>3.2930000000000001</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43">
         <v>2250.665</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43">
         <v>22.515999999999998</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43">
         <v>2.1819999999999999</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H43">
         <v>20.334</v>
       </c>
-      <c r="I43" s="6">
+      <c r="I43">
         <v>199.9</v>
       </c>
-      <c r="J43" s="6">
+      <c r="J43">
         <v>2071.0990000000002</v>
       </c>
-      <c r="K43" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L43" s="6">
+      <c r="K43" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43">
         <v>2071.0990000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A44" s="2">
         <v>1980</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44">
         <v>2286.4389999999999</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="6">
+      <c r="C44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44">
         <v>3.161</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44">
         <v>2289.6</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44">
         <v>25.021000000000001</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44">
         <v>4.0960000000000001</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44">
         <v>20.925999999999998</v>
       </c>
-      <c r="I44" s="6">
+      <c r="I44">
         <v>216.077</v>
       </c>
-      <c r="J44" s="6">
+      <c r="J44">
         <v>2094.4490000000001</v>
       </c>
-      <c r="K44" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L44" s="6">
+      <c r="K44" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44">
         <v>2094.4490000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A45" s="2">
         <v>1981</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45">
         <v>2294.8119999999999</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="6">
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45">
         <v>3.161</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45">
         <v>2297.973</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45">
         <v>36.298000000000002</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45">
         <v>3.06</v>
       </c>
-      <c r="H45" s="6">
+      <c r="H45">
         <v>33.237000000000002</v>
       </c>
-      <c r="I45" s="6">
+      <c r="I45">
         <v>184.108</v>
       </c>
-      <c r="J45" s="6">
+      <c r="J45">
         <v>2147.1030000000001</v>
       </c>
-      <c r="K45" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L45" s="6">
+      <c r="K45" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45">
         <v>2147.1030000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A46" s="2">
         <v>1982</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46">
         <v>2241.2109999999998</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="6">
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46">
         <v>3.161</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46">
         <v>2244.3719999999998</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46">
         <v>32.851999999999997</v>
       </c>
-      <c r="G46" s="6">
+      <c r="G46">
         <v>3.536</v>
       </c>
-      <c r="H46" s="6">
+      <c r="H46">
         <v>29.315999999999999</v>
       </c>
-      <c r="I46" s="6">
+      <c r="I46">
         <v>187.24700000000001</v>
       </c>
-      <c r="J46" s="6">
+      <c r="J46">
         <v>2086.4409999999998</v>
       </c>
-      <c r="K46" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" s="6">
+      <c r="K46" t="s">
+        <v>19</v>
+      </c>
+      <c r="L46">
         <v>2086.4409999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A47" s="2">
         <v>1983</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47">
         <v>2310.2849999999999</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="6">
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47">
         <v>3.161</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47">
         <v>2313.4459999999999</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47">
         <v>38.667999999999999</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G47">
         <v>3.3370000000000002</v>
       </c>
-      <c r="H47" s="6">
+      <c r="H47">
         <v>35.33</v>
       </c>
-      <c r="I47" s="6">
+      <c r="I47">
         <v>197.821</v>
       </c>
-      <c r="J47" s="6">
+      <c r="J47">
         <v>2150.9549999999999</v>
       </c>
-      <c r="K47" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L47" s="6">
+      <c r="K47" t="s">
+        <v>19</v>
+      </c>
+      <c r="L47">
         <v>2150.9549999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A48" s="2">
         <v>1984</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48">
         <v>2416.3040000000001</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" s="6">
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48">
         <v>3.161</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48">
         <v>2419.4650000000001</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48">
         <v>42.219000000000001</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G48">
         <v>2.5579999999999998</v>
       </c>
-      <c r="H48" s="6">
+      <c r="H48">
         <v>39.661000000000001</v>
       </c>
-      <c r="I48" s="6">
+      <c r="I48">
         <v>173.33</v>
       </c>
-      <c r="J48" s="6">
+      <c r="J48">
         <v>2285.7959999999998</v>
       </c>
-      <c r="K48" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="6">
+      <c r="K48" t="s">
+        <v>19</v>
+      </c>
+      <c r="L48">
         <v>2285.7959999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A49" s="2">
         <v>1985</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49">
         <v>2469.8409999999999</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="6">
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49">
         <v>3.161</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49">
         <v>2473.002</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49">
         <v>45.895000000000003</v>
       </c>
-      <c r="G49" s="6">
+      <c r="G49">
         <v>4.9649999999999999</v>
       </c>
-      <c r="H49" s="6">
+      <c r="H49">
         <v>40.930999999999997</v>
       </c>
-      <c r="I49" s="6">
+      <c r="I49">
         <v>189.959</v>
       </c>
-      <c r="J49" s="6">
+      <c r="J49">
         <v>2323.9740000000002</v>
       </c>
-      <c r="K49" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L49" s="6">
+      <c r="K49" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49">
         <v>2323.9740000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A50" s="2">
         <v>1986</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50">
         <v>2487.31</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="6">
+      <c r="C50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50">
         <v>3.161</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50">
         <v>2490.471</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50">
         <v>40.713000000000001</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G50">
         <v>4.8159999999999998</v>
       </c>
-      <c r="H50" s="6">
+      <c r="H50">
         <v>35.896999999999998</v>
       </c>
-      <c r="I50" s="6">
+      <c r="I50">
         <v>157.61500000000001</v>
       </c>
-      <c r="J50" s="6">
+      <c r="J50">
         <v>2368.7530000000002</v>
       </c>
-      <c r="K50" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L50" s="6">
+      <c r="K50" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50">
         <v>2368.7530000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A51" s="2">
         <v>1987</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51">
         <v>2572.127</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D51" s="6">
+      <c r="C51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51">
         <v>3.161</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51">
         <v>2575.288</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F51">
         <v>52.219000000000001</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51">
         <v>5.8819999999999997</v>
       </c>
-      <c r="H51" s="6">
+      <c r="H51">
         <v>46.337000000000003</v>
       </c>
-      <c r="I51" s="6">
+      <c r="I51">
         <v>164.352</v>
       </c>
-      <c r="J51" s="6">
+      <c r="J51">
         <v>2457.2719999999999</v>
       </c>
-      <c r="K51" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="6">
+      <c r="K51" t="s">
+        <v>19</v>
+      </c>
+      <c r="L51">
         <v>2457.2719999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A52" s="2">
         <v>1988</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52">
         <v>2704.25</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="6">
+      <c r="C52" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52">
         <v>3.161</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52">
         <v>2707.4110000000001</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52">
         <v>38.837000000000003</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G52">
         <v>7.0670000000000002</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H52">
         <v>31.77</v>
       </c>
-      <c r="I52" s="6">
+      <c r="I52">
         <v>161.119</v>
       </c>
-      <c r="J52" s="6">
+      <c r="J52">
         <v>2578.0619999999999</v>
       </c>
-      <c r="K52" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L52" s="6">
+      <c r="K52" t="s">
+        <v>19</v>
+      </c>
+      <c r="L52">
         <v>2578.0619999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A53" s="2">
         <v>1989</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53">
         <v>2848.2269999999999</v>
       </c>
-      <c r="C53" s="6">
+      <c r="C53">
         <v>4.2510000000000003</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53">
         <v>114.828</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53">
         <v>2967.1460000000002</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F53">
         <v>26.11</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G53">
         <v>15.135</v>
       </c>
-      <c r="H53" s="6">
+      <c r="H53">
         <v>10.976000000000001</v>
       </c>
-      <c r="I53" s="6">
+      <c r="I53">
         <v>222.48699999999999</v>
       </c>
-      <c r="J53" s="6">
+      <c r="J53">
         <v>2646.8090000000002</v>
       </c>
-      <c r="K53" s="6">
+      <c r="K53">
         <v>108.82599999999999</v>
       </c>
-      <c r="L53" s="6">
+      <c r="L53">
         <v>2755.6350000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A54" s="2">
         <v>1990</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54">
         <v>2901.3220000000001</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C54">
         <v>5.8369999999999997</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54">
         <v>130.83000000000001</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54">
         <v>3037.8270000000002</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54">
         <v>18.445</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54">
         <v>16.134</v>
       </c>
-      <c r="H54" s="6">
+      <c r="H54">
         <v>2.3119999999999998</v>
       </c>
-      <c r="I54" s="6">
+      <c r="I54">
         <v>203.05600000000001</v>
       </c>
-      <c r="J54" s="6">
+      <c r="J54">
         <v>2712.5549999999998</v>
       </c>
-      <c r="K54" s="6">
+      <c r="K54">
         <v>124.529</v>
       </c>
-      <c r="L54" s="6">
+      <c r="L54">
         <v>2837.0839999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A55" s="2">
         <v>1991</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55">
         <v>2935.5610000000001</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C55">
         <v>5.6589999999999998</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55">
         <v>132.57900000000001</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55">
         <v>3073.799</v>
       </c>
-      <c r="F55" s="6">
+      <c r="F55">
         <v>21.931000000000001</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G55">
         <v>2.3050000000000002</v>
       </c>
-      <c r="H55" s="6">
+      <c r="H55">
         <v>19.626000000000001</v>
       </c>
-      <c r="I55" s="6">
+      <c r="I55">
         <v>207.36500000000001</v>
       </c>
-      <c r="J55" s="6">
+      <c r="J55">
         <v>2762.0030000000002</v>
       </c>
-      <c r="K55" s="6">
+      <c r="K55">
         <v>124.057</v>
       </c>
-      <c r="L55" s="6">
+      <c r="L55">
         <v>2886.06</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A56" s="2">
         <v>1992</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56">
         <v>2934.3739999999998</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56">
         <v>6.2279999999999998</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56">
         <v>143.28</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56">
         <v>3083.8820000000001</v>
       </c>
-      <c r="F56" s="6">
+      <c r="F56">
         <v>28.247</v>
       </c>
-      <c r="G56" s="6">
+      <c r="G56">
         <v>2.827</v>
       </c>
-      <c r="H56" s="6">
+      <c r="H56">
         <v>25.42</v>
       </c>
-      <c r="I56" s="6">
+      <c r="I56">
         <v>212.096</v>
       </c>
-      <c r="J56" s="6">
+      <c r="J56">
         <v>2763.3649999999998</v>
       </c>
-      <c r="K56" s="6">
+      <c r="K56">
         <v>133.84100000000001</v>
       </c>
-      <c r="L56" s="6">
+      <c r="L56">
         <v>2897.2069999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A57" s="2">
         <v>1993</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57">
         <v>3043.8969999999999</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C57">
         <v>7</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57">
         <v>146.29400000000001</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57">
         <v>3197.1909999999998</v>
       </c>
-      <c r="F57" s="6">
+      <c r="F57">
         <v>31.358000000000001</v>
       </c>
-      <c r="G57" s="6">
+      <c r="G57">
         <v>3.5409999999999999</v>
       </c>
-      <c r="H57" s="6">
+      <c r="H57">
         <v>27.817</v>
       </c>
-      <c r="I57" s="6">
+      <c r="I57">
         <v>224.30799999999999</v>
       </c>
-      <c r="J57" s="6">
+      <c r="J57">
         <v>2861.462</v>
       </c>
-      <c r="K57" s="6">
+      <c r="K57">
         <v>139.238</v>
       </c>
-      <c r="L57" s="6">
+      <c r="L57">
         <v>3000.7</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A58" s="2">
         <v>1994</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58">
         <v>3088.7249999999999</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C58">
         <v>7.6189999999999998</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58">
         <v>151.178</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E58">
         <v>3247.5219999999999</v>
       </c>
-      <c r="F58" s="6">
+      <c r="F58">
         <v>46.832999999999998</v>
       </c>
-      <c r="G58" s="6">
+      <c r="G58">
         <v>2.0099999999999998</v>
       </c>
-      <c r="H58" s="6">
+      <c r="H58">
         <v>44.823</v>
       </c>
-      <c r="I58" s="6">
+      <c r="I58">
         <v>211.45699999999999</v>
       </c>
-      <c r="J58" s="6">
+      <c r="J58">
         <v>2934.5630000000001</v>
       </c>
-      <c r="K58" s="6">
+      <c r="K58">
         <v>146.32499999999999</v>
       </c>
-      <c r="L58" s="6">
+      <c r="L58">
         <v>3080.8879999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A59" s="2">
         <v>1995</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59">
         <v>3194.23</v>
       </c>
-      <c r="C59" s="6">
+      <c r="C59">
         <v>8.2319999999999993</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D59">
         <v>151.02500000000001</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59">
         <v>3353.4870000000001</v>
       </c>
-      <c r="F59" s="6">
+      <c r="F59">
         <v>42.853999999999999</v>
       </c>
-      <c r="G59" s="6">
+      <c r="G59">
         <v>3.6230000000000002</v>
       </c>
-      <c r="H59" s="6">
+      <c r="H59">
         <v>39.231000000000002</v>
       </c>
-      <c r="I59" s="6">
+      <c r="I59">
         <v>228.755</v>
       </c>
-      <c r="J59" s="6">
+      <c r="J59">
         <v>3013.2869999999998</v>
       </c>
-      <c r="K59" s="6">
+      <c r="K59">
         <v>150.67699999999999</v>
       </c>
-      <c r="L59" s="6">
+      <c r="L59">
         <v>3163.9630000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="7">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A60" s="2">
         <v>1996</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60">
         <v>3284.1410000000001</v>
       </c>
-      <c r="C60" s="6">
+      <c r="C60">
         <v>9.0299999999999994</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D60">
         <v>151.017</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E60">
         <v>3444.1880000000001</v>
       </c>
-      <c r="F60" s="6">
+      <c r="F60">
         <v>43.497</v>
       </c>
-      <c r="G60" s="6">
+      <c r="G60">
         <v>3.302</v>
       </c>
-      <c r="H60" s="6">
+      <c r="H60">
         <v>40.195</v>
       </c>
-      <c r="I60" s="6">
+      <c r="I60">
         <v>230.61699999999999</v>
       </c>
-      <c r="J60" s="6">
+      <c r="J60">
         <v>3101.127</v>
       </c>
-      <c r="K60" s="6">
+      <c r="K60">
         <v>152.63800000000001</v>
       </c>
-      <c r="L60" s="6">
+      <c r="L60">
         <v>3253.7649999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="7">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A61" s="2">
         <v>1997</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61">
         <v>3329.375</v>
       </c>
-      <c r="C61" s="6">
+      <c r="C61">
         <v>8.7010000000000005</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D61">
         <v>154.09700000000001</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61">
         <v>3492.172</v>
       </c>
-      <c r="F61" s="6">
+      <c r="F61">
         <v>43.030999999999999</v>
       </c>
-      <c r="G61" s="6">
+      <c r="G61">
         <v>8.9740000000000002</v>
       </c>
-      <c r="H61" s="6">
+      <c r="H61">
         <v>34.057000000000002</v>
       </c>
-      <c r="I61" s="6">
+      <c r="I61">
         <v>224.38</v>
       </c>
-      <c r="J61" s="6">
+      <c r="J61">
         <v>3145.61</v>
       </c>
-      <c r="K61" s="6">
+      <c r="K61">
         <v>156.239</v>
       </c>
-      <c r="L61" s="6">
+      <c r="L61">
         <v>3301.8490000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="7">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A62" s="2">
         <v>1998</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62">
         <v>3457.4160000000002</v>
       </c>
-      <c r="C62" s="6">
+      <c r="C62">
         <v>8.7479999999999993</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D62">
         <v>154.13200000000001</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E62">
         <v>3620.2950000000001</v>
       </c>
-      <c r="F62" s="6">
+      <c r="F62">
         <v>39.512999999999998</v>
       </c>
-      <c r="G62" s="6">
+      <c r="G62">
         <v>13.656000000000001</v>
       </c>
-      <c r="H62" s="6">
+      <c r="H62">
         <v>25.856999999999999</v>
       </c>
-      <c r="I62" s="6">
+      <c r="I62">
         <v>221.05600000000001</v>
       </c>
-      <c r="J62" s="6">
+      <c r="J62">
         <v>3264.2310000000002</v>
       </c>
-      <c r="K62" s="6">
+      <c r="K62">
         <v>160.86600000000001</v>
       </c>
-      <c r="L62" s="6">
+      <c r="L62">
         <v>3425.0970000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="7">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A63" s="2">
         <v>1999</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63">
         <v>3529.982</v>
       </c>
-      <c r="C63" s="6">
+      <c r="C63">
         <v>8.5630000000000006</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D63">
         <v>156.26400000000001</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E63">
         <v>3694.81</v>
       </c>
-      <c r="F63" s="6">
+      <c r="F63">
         <v>43.215000000000003</v>
       </c>
-      <c r="G63" s="6">
+      <c r="G63">
         <v>14.222</v>
       </c>
-      <c r="H63" s="6">
+      <c r="H63">
         <v>28.992999999999999</v>
       </c>
-      <c r="I63" s="6">
+      <c r="I63">
         <v>240.08600000000001</v>
       </c>
-      <c r="J63" s="6">
+      <c r="J63">
         <v>3312.087</v>
       </c>
-      <c r="K63" s="6">
+      <c r="K63">
         <v>171.62899999999999</v>
       </c>
-      <c r="L63" s="6">
+      <c r="L63">
         <v>3483.7159999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="7">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A64" s="2">
         <v>2000</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64">
         <v>3637.529</v>
       </c>
-      <c r="C64" s="6">
+      <c r="C64">
         <v>7.9029999999999996</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64">
         <v>156.673</v>
       </c>
-      <c r="E64" s="6">
+      <c r="E64">
         <v>3802.105</v>
       </c>
-      <c r="F64" s="6">
+      <c r="F64">
         <v>48.591999999999999</v>
       </c>
-      <c r="G64" s="6">
+      <c r="G64">
         <v>14.829000000000001</v>
       </c>
-      <c r="H64" s="6">
+      <c r="H64">
         <v>33.762999999999998</v>
       </c>
-      <c r="I64" s="6">
+      <c r="I64">
         <v>243.511</v>
       </c>
-      <c r="J64" s="6">
+      <c r="J64">
         <v>3421.4140000000002</v>
       </c>
-      <c r="K64" s="6">
+      <c r="K64">
         <v>170.94300000000001</v>
       </c>
-      <c r="L64" s="6">
+      <c r="L64">
         <v>3592.357</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="7">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A65" s="2">
         <v>2001</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65">
         <v>3580.0529999999999</v>
       </c>
-      <c r="C65" s="6">
+      <c r="C65">
         <v>7.4160000000000004</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D65">
         <v>149.17500000000001</v>
       </c>
-      <c r="E65" s="6">
+      <c r="E65">
         <v>3736.6439999999998</v>
       </c>
-      <c r="F65" s="6">
+      <c r="F65">
         <v>38.5</v>
       </c>
-      <c r="G65" s="6">
+      <c r="G65">
         <v>16.472999999999999</v>
       </c>
-      <c r="H65" s="6">
+      <c r="H65">
         <v>22.027000000000001</v>
       </c>
-      <c r="I65" s="6">
+      <c r="I65">
         <v>201.56399999999999</v>
       </c>
-      <c r="J65" s="6">
+      <c r="J65">
         <v>3394.4580000000001</v>
       </c>
-      <c r="K65" s="6">
+      <c r="K65">
         <v>162.649</v>
       </c>
-      <c r="L65" s="6">
+      <c r="L65">
         <v>3557.107</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="7">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A66" s="2">
         <v>2002</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66">
         <v>3698.4580000000001</v>
       </c>
-      <c r="C66" s="6">
+      <c r="C66">
         <v>7.415</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66">
         <v>152.58000000000001</v>
       </c>
-      <c r="E66" s="6">
+      <c r="E66">
         <v>3858.4520000000002</v>
       </c>
-      <c r="F66" s="6">
+      <c r="F66">
         <v>36.779000000000003</v>
       </c>
-      <c r="G66" s="6">
+      <c r="G66">
         <v>15.795999999999999</v>
       </c>
-      <c r="H66" s="6">
+      <c r="H66">
         <v>20.983000000000001</v>
       </c>
-      <c r="I66" s="6">
+      <c r="I66">
         <v>247.785</v>
       </c>
-      <c r="J66" s="6">
+      <c r="J66">
         <v>3465.4659999999999</v>
       </c>
-      <c r="K66" s="6">
+      <c r="K66">
         <v>166.184</v>
       </c>
-      <c r="L66" s="6">
+      <c r="L66">
         <v>3631.65</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="7">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A67" s="2">
         <v>2003</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67">
         <v>3721.1590000000001</v>
       </c>
-      <c r="C67" s="6">
+      <c r="C67">
         <v>7.4960000000000004</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D67">
         <v>154.53</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E67">
         <v>3883.1849999999999</v>
       </c>
-      <c r="F67" s="6">
+      <c r="F67">
         <v>30.395</v>
       </c>
-      <c r="G67" s="6">
+      <c r="G67">
         <v>23.975000000000001</v>
       </c>
-      <c r="H67" s="6">
+      <c r="H67">
         <v>6.42</v>
       </c>
-      <c r="I67" s="6">
+      <c r="I67">
         <v>227.57599999999999</v>
       </c>
-      <c r="J67" s="6">
+      <c r="J67">
         <v>3493.7339999999999</v>
       </c>
-      <c r="K67" s="6">
+      <c r="K67">
         <v>168.29499999999999</v>
       </c>
-      <c r="L67" s="6">
+      <c r="L67">
         <v>3662.029</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="7">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A68" s="2">
         <v>2004</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68">
         <v>3808.36</v>
       </c>
-      <c r="C68" s="6">
+      <c r="C68">
         <v>8.27</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68">
         <v>153.92500000000001</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E68">
         <v>3970.5549999999998</v>
       </c>
-      <c r="F68" s="6">
+      <c r="F68">
         <v>34.21</v>
       </c>
-      <c r="G68" s="6">
+      <c r="G68">
         <v>22.898</v>
       </c>
-      <c r="H68" s="6">
+      <c r="H68">
         <v>11.311999999999999</v>
       </c>
-      <c r="I68" s="6">
+      <c r="I68">
         <v>265.91800000000001</v>
       </c>
-      <c r="J68" s="6">
+      <c r="J68">
         <v>3547.4789999999998</v>
       </c>
-      <c r="K68" s="6">
+      <c r="K68">
         <v>168.47</v>
       </c>
-      <c r="L68" s="6">
+      <c r="L68">
         <v>3715.9490000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="7">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A69" s="2">
         <v>2005</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69">
         <v>3902.192</v>
       </c>
-      <c r="C69" s="6">
+      <c r="C69">
         <v>8.4920000000000009</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D69">
         <v>144.739</v>
       </c>
-      <c r="E69" s="6">
+      <c r="E69">
         <v>4055.4229999999998</v>
       </c>
-      <c r="F69" s="6">
+      <c r="F69">
         <v>43.929000000000002</v>
       </c>
-      <c r="G69" s="6">
+      <c r="G69">
         <v>19.151</v>
       </c>
-      <c r="H69" s="6">
+      <c r="H69">
         <v>24.777999999999999</v>
       </c>
-      <c r="I69" s="6">
+      <c r="I69">
         <v>269.21699999999998</v>
       </c>
-      <c r="J69" s="6">
+      <c r="J69">
         <v>3660.9690000000001</v>
       </c>
-      <c r="K69" s="6">
+      <c r="K69">
         <v>150.01599999999999</v>
       </c>
-      <c r="L69" s="6">
+      <c r="L69">
         <v>3810.9839999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="7">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A70" s="2">
         <v>2006</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70">
         <v>3908.0770000000002</v>
       </c>
-      <c r="C70" s="6">
+      <c r="C70">
         <v>8.3710000000000004</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70">
         <v>148.25399999999999</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E70">
         <v>4064.7020000000002</v>
       </c>
-      <c r="F70" s="6">
+      <c r="F70">
         <v>42.691000000000003</v>
       </c>
-      <c r="G70" s="6">
+      <c r="G70">
         <v>24.271000000000001</v>
       </c>
-      <c r="H70" s="6">
+      <c r="H70">
         <v>18.420000000000002</v>
       </c>
-      <c r="I70" s="6">
+      <c r="I70">
         <v>266.27699999999999</v>
       </c>
-      <c r="J70" s="6">
+      <c r="J70">
         <v>3669.9189999999999</v>
       </c>
-      <c r="K70" s="6">
+      <c r="K70">
         <v>146.92699999999999</v>
       </c>
-      <c r="L70" s="6">
+      <c r="L70">
         <v>3816.8449999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="7">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A71" s="2">
         <v>2007</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71">
         <v>4005.3429999999998</v>
       </c>
-      <c r="C71" s="6">
+      <c r="C71">
         <v>8.2729999999999997</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71">
         <v>143.12799999999999</v>
       </c>
-      <c r="E71" s="6">
+      <c r="E71">
         <v>4156.7449999999999</v>
       </c>
-      <c r="F71" s="6">
+      <c r="F71">
         <v>51.396000000000001</v>
       </c>
-      <c r="G71" s="6">
+      <c r="G71">
         <v>20.143999999999998</v>
       </c>
-      <c r="H71" s="6">
+      <c r="H71">
         <v>31.251999999999999</v>
       </c>
-      <c r="I71" s="6">
+      <c r="I71">
         <v>297.76600000000002</v>
       </c>
-      <c r="J71" s="6">
+      <c r="J71">
         <v>3764.5610000000001</v>
       </c>
-      <c r="K71" s="6">
+      <c r="K71">
         <v>125.67</v>
       </c>
-      <c r="L71" s="6">
+      <c r="L71">
         <v>3890.2310000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="7">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A72" s="2">
         <v>2008</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72">
         <v>3974.3490000000002</v>
       </c>
-      <c r="C72" s="6">
+      <c r="C72">
         <v>7.9260000000000002</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72">
         <v>137.113</v>
       </c>
-      <c r="E72" s="6">
+      <c r="E72">
         <v>4119.3879999999999</v>
       </c>
-      <c r="F72" s="6">
+      <c r="F72">
         <v>57.018999999999998</v>
       </c>
-      <c r="G72" s="6">
+      <c r="G72">
         <v>24.198</v>
       </c>
-      <c r="H72" s="6">
+      <c r="H72">
         <v>32.820999999999998</v>
       </c>
-      <c r="I72" s="6">
+      <c r="I72">
         <v>286.048</v>
       </c>
-      <c r="J72" s="6">
+      <c r="J72">
         <v>3733.9650000000001</v>
       </c>
-      <c r="K72" s="6">
+      <c r="K72">
         <v>132.197</v>
       </c>
-      <c r="L72" s="6">
+      <c r="L72">
         <v>3866.1610000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="7">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A73" s="2">
         <v>2009</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73">
         <v>3809.837</v>
       </c>
-      <c r="C73" s="6">
+      <c r="C73">
         <v>8.1649999999999991</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73">
         <v>132.32900000000001</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E73">
         <v>3950.3310000000001</v>
       </c>
-      <c r="F73" s="6">
+      <c r="F73">
         <v>52.191000000000003</v>
       </c>
-      <c r="G73" s="6">
+      <c r="G73">
         <v>18.138000000000002</v>
       </c>
-      <c r="H73" s="6">
+      <c r="H73">
         <v>34.052999999999997</v>
       </c>
-      <c r="I73" s="6">
+      <c r="I73">
         <v>260.64999999999998</v>
       </c>
-      <c r="J73" s="6">
+      <c r="J73">
         <v>3596.7950000000001</v>
       </c>
-      <c r="K73" s="6">
+      <c r="K73">
         <v>126.938</v>
       </c>
-      <c r="L73" s="6">
+      <c r="L73">
         <v>3723.7330000000002</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="7">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A74" s="2">
         <v>2010</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74">
         <v>3972.386</v>
       </c>
-      <c r="C74" s="6">
+      <c r="C74">
         <v>8.5920000000000005</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74">
         <v>144.08199999999999</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E74">
         <v>4125.0600000000004</v>
       </c>
-      <c r="F74" s="6">
+      <c r="F74">
         <v>45.082999999999998</v>
       </c>
-      <c r="G74" s="6">
+      <c r="G74">
         <v>19.106000000000002</v>
       </c>
-      <c r="H74" s="6">
+      <c r="H74">
         <v>25.977</v>
       </c>
-      <c r="I74" s="6">
+      <c r="I74">
         <v>264.28500000000003</v>
       </c>
-      <c r="J74" s="6">
+      <c r="J74">
         <v>3754.8409999999999</v>
       </c>
-      <c r="K74" s="6">
+      <c r="K74">
         <v>131.91</v>
       </c>
-      <c r="L74" s="6">
+      <c r="L74">
         <v>3886.752</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="7">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A75" s="2">
         <v>2011</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75">
         <v>3948.1860000000001</v>
       </c>
-      <c r="C75" s="6">
+      <c r="C75">
         <v>10.08</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D75">
         <v>141.875</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E75">
         <v>4100.1409999999996</v>
       </c>
-      <c r="F75" s="6">
+      <c r="F75">
         <v>52.3</v>
       </c>
-      <c r="G75" s="6">
+      <c r="G75">
         <v>15.048999999999999</v>
       </c>
-      <c r="H75" s="6">
+      <c r="H75">
         <v>37.250999999999998</v>
       </c>
-      <c r="I75" s="6">
+      <c r="I75">
         <v>254.792</v>
       </c>
-      <c r="J75" s="6">
+      <c r="J75">
         <v>3749.846</v>
       </c>
-      <c r="K75" s="6">
+      <c r="K75">
         <v>132.75399999999999</v>
       </c>
-      <c r="L75" s="6">
+      <c r="L75">
         <v>3882.6</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="7">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A76" s="2">
         <v>2012</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76">
         <v>3890.3580000000002</v>
       </c>
-      <c r="C76" s="6">
+      <c r="C76">
         <v>11.301</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D76">
         <v>146.107</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76">
         <v>4047.7649999999999</v>
       </c>
-      <c r="F76" s="6">
+      <c r="F76">
         <v>59.256999999999998</v>
       </c>
-      <c r="G76" s="6">
+      <c r="G76">
         <v>11.996</v>
       </c>
-      <c r="H76" s="6">
+      <c r="H76">
         <v>47.261000000000003</v>
       </c>
-      <c r="I76" s="6">
+      <c r="I76">
         <v>262.72000000000003</v>
       </c>
-      <c r="J76" s="6">
+      <c r="J76">
         <v>3694.65</v>
       </c>
-      <c r="K76" s="6">
+      <c r="K76">
         <v>137.65700000000001</v>
       </c>
-      <c r="L76" s="6">
+      <c r="L76">
         <v>3832.306</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="7">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A77" s="2">
         <v>2013</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77">
         <v>3903.7150000000001</v>
       </c>
-      <c r="C77" s="6">
+      <c r="C77">
         <v>12.234</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D77">
         <v>150.01499999999999</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E77">
         <v>4065.9639999999999</v>
       </c>
-      <c r="F77" s="6">
+      <c r="F77">
         <v>69.248999999999995</v>
       </c>
-      <c r="G77" s="6">
+      <c r="G77">
         <v>11.372999999999999</v>
       </c>
-      <c r="H77" s="6">
+      <c r="H77">
         <v>57.875999999999998</v>
       </c>
-      <c r="I77" s="6">
+      <c r="I77">
         <v>255.51</v>
       </c>
-      <c r="J77" s="6">
+      <c r="J77">
         <v>3724.8679999999999</v>
       </c>
-      <c r="K77" s="6">
+      <c r="K77">
         <v>143.46199999999999</v>
       </c>
-      <c r="L77" s="6">
+      <c r="L77">
         <v>3868.33</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="7">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A78" s="2">
         <v>2014</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78">
         <v>3937.0030000000002</v>
       </c>
-      <c r="C78" s="6">
+      <c r="C78">
         <v>12.52</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D78">
         <v>144.083</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78">
         <v>4093.6060000000002</v>
       </c>
-      <c r="F78" s="6">
+      <c r="F78">
         <v>66.510000000000005</v>
       </c>
-      <c r="G78" s="6">
+      <c r="G78">
         <v>13.298</v>
       </c>
-      <c r="H78" s="6">
+      <c r="H78">
         <v>53.212000000000003</v>
       </c>
-      <c r="I78" s="6">
+      <c r="I78">
         <v>243.54400000000001</v>
       </c>
-      <c r="J78" s="6">
+      <c r="J78">
         <v>3764.7</v>
       </c>
-      <c r="K78" s="6">
+      <c r="K78">
         <v>138.57400000000001</v>
       </c>
-      <c r="L78" s="6">
+      <c r="L78">
         <v>3903.2739999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="7">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A79" s="2">
         <v>2015</v>
       </c>
-      <c r="B79" s="6">
-        <v>3930.5790000000002</v>
-      </c>
-      <c r="C79" s="6">
-        <v>13.029</v>
-      </c>
-      <c r="D79" s="6">
-        <v>143.773</v>
-      </c>
-      <c r="E79" s="6">
-        <v>4087.3809999999999</v>
-      </c>
-      <c r="F79" s="6">
-        <v>75.602999999999994</v>
-      </c>
-      <c r="G79" s="6">
-        <v>9.1449999999999996</v>
-      </c>
-      <c r="H79" s="6">
-        <v>66.457999999999998</v>
-      </c>
-      <c r="I79" s="6">
-        <v>290.56400000000002</v>
-      </c>
-      <c r="J79" s="6">
-        <v>3724.5250000000001</v>
-      </c>
-      <c r="K79" s="6">
-        <v>138.75</v>
-      </c>
-      <c r="L79" s="6">
-        <v>3863.2750000000001</v>
+      <c r="B79">
+        <v>3919.2939999999999</v>
+      </c>
+      <c r="C79">
+        <v>12.595000000000001</v>
+      </c>
+      <c r="D79">
+        <v>145.71199999999999</v>
+      </c>
+      <c r="E79">
+        <v>4077.6010000000001</v>
+      </c>
+      <c r="F79">
+        <v>75.77</v>
+      </c>
+      <c r="G79">
+        <v>9.1</v>
+      </c>
+      <c r="H79">
+        <v>66.671000000000006</v>
+      </c>
+      <c r="I79">
+        <v>244.11199999999999</v>
+      </c>
+      <c r="J79">
+        <v>3758.9920000000002</v>
+      </c>
+      <c r="K79">
+        <v>141.16800000000001</v>
+      </c>
+      <c r="L79">
+        <v>3900.16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A80" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B80">
+        <v>3918.078</v>
+      </c>
+      <c r="C80">
+        <v>12.706</v>
+      </c>
+      <c r="D80">
+        <v>145.88999999999999</v>
+      </c>
+      <c r="E80">
+        <v>4076.6750000000002</v>
+      </c>
+      <c r="F80">
+        <v>72.715999999999994</v>
+      </c>
+      <c r="G80">
+        <v>6.2140000000000004</v>
+      </c>
+      <c r="H80">
+        <v>66.501999999999995</v>
+      </c>
+      <c r="I80">
+        <v>240.87100000000001</v>
+      </c>
+      <c r="J80">
+        <v>3762.462</v>
+      </c>
+      <c r="K80">
+        <v>139.84399999999999</v>
+      </c>
+      <c r="L80">
+        <v>3902.306</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A81" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B81">
+        <v>3877.453</v>
+      </c>
+      <c r="C81">
+        <v>13.06</v>
+      </c>
+      <c r="D81">
+        <v>143.75800000000001</v>
+      </c>
+      <c r="E81">
+        <v>4034.2710000000002</v>
+      </c>
+      <c r="F81">
+        <v>65.685000000000002</v>
+      </c>
+      <c r="G81">
+        <v>9.3710000000000004</v>
+      </c>
+      <c r="H81">
+        <v>56.314</v>
+      </c>
+      <c r="I81">
+        <v>226.114</v>
+      </c>
+      <c r="J81">
+        <v>3723.3560000000002</v>
+      </c>
+      <c r="K81">
+        <v>141.114</v>
+      </c>
+      <c r="L81">
+        <v>3864.47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A82" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B82">
+        <v>4017.9659999999999</v>
+      </c>
+      <c r="C82">
+        <v>13.311999999999999</v>
+      </c>
+      <c r="D82">
+        <v>146.798</v>
+      </c>
+      <c r="E82">
+        <v>4178.0770000000002</v>
+      </c>
+      <c r="F82">
+        <v>58.261000000000003</v>
+      </c>
+      <c r="G82">
+        <v>13.804</v>
+      </c>
+      <c r="H82">
+        <v>44.456000000000003</v>
+      </c>
+      <c r="I82">
+        <v>219.23400000000001</v>
+      </c>
+      <c r="J82">
+        <v>3859.1849999999999</v>
+      </c>
+      <c r="K82">
+        <v>144.114</v>
+      </c>
+      <c r="L82">
+        <v>4003.299</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A83" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B83">
+        <v>3955.7809999999999</v>
+      </c>
+      <c r="C83">
+        <v>13.624000000000001</v>
+      </c>
+      <c r="D83">
+        <v>148.64500000000001</v>
+      </c>
+      <c r="E83">
+        <v>4118.0510000000004</v>
+      </c>
+      <c r="F83">
+        <v>59.052</v>
+      </c>
+      <c r="G83">
+        <v>20.007999999999999</v>
+      </c>
+      <c r="H83">
+        <v>39.043999999999997</v>
+      </c>
+      <c r="I83">
+        <v>261.5</v>
+      </c>
+      <c r="J83">
+        <v>3749.538</v>
+      </c>
+      <c r="K83">
+        <v>146.05699999999999</v>
+      </c>
+      <c r="L83">
+        <v>3895.5949999999998</v>
       </c>
     </row>
   </sheetData>
@@ -3468,30 +3635,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.265625" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>2000</v>
       </c>
@@ -3508,7 +3677,7 @@
         <v>6.6944071098814603E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2001</v>
       </c>
@@ -3525,7 +3694,7 @@
         <v>5.6301959775455837E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2002</v>
       </c>
@@ -3542,7 +3711,7 @@
         <v>6.69968403047973E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>2003</v>
       </c>
@@ -3559,7 +3728,7 @@
         <v>6.1157289973365822E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>2004</v>
       </c>
@@ -3576,7 +3745,7 @@
         <v>6.9824806478379145E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>2005</v>
       </c>
@@ -3593,7 +3762,7 @@
         <v>6.8991223394440859E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>2006</v>
       </c>
@@ -3610,7 +3779,7 @@
         <v>6.8135044422103247E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>2007</v>
       </c>
@@ -3627,7 +3796,7 @@
         <v>7.4342197409809851E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>2008</v>
       </c>
@@ -3644,7 +3813,7 @@
         <v>7.1973548372324628E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>2009</v>
       </c>
@@ -3661,7 +3830,7 @@
         <v>6.8415000431776993E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>2010</v>
       </c>
@@ -3678,7 +3847,7 @@
         <v>6.6530543607796436E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>2011</v>
       </c>
@@ -3695,7 +3864,7 @@
         <v>6.4533940396931652E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>2012</v>
       </c>
@@ -3712,7 +3881,7 @@
         <v>6.7531060123515632E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>2013</v>
       </c>
@@ -3729,7 +3898,7 @@
         <v>6.5453036402503759E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>2014</v>
       </c>
@@ -3746,37 +3915,105 @@
         <v>6.18602525829927E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>2015</v>
       </c>
       <c r="B17" s="5">
         <f>'MER 7.1'!I79</f>
-        <v>290.56400000000002</v>
+        <v>244.11199999999999</v>
       </c>
       <c r="C17" s="5">
         <f>'MER 7.1'!B79</f>
-        <v>3930.5790000000002</v>
+        <v>3919.2939999999999</v>
       </c>
       <c r="D17" s="4">
         <f>B17/C17</f>
-        <v>7.3923968962333539E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="13">
-        <f>AVERAGE(D2:D17)</f>
-        <v>6.7057173983583865E-2</v>
+        <v>6.2284686986993069E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B18" s="5">
+        <f>'MER 7.1'!I80</f>
+        <v>240.87100000000001</v>
+      </c>
+      <c r="C18" s="5">
+        <f>'MER 7.1'!B80</f>
+        <v>3918.078</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" ref="D18:D21" si="2">B18/C18</f>
+        <v>6.1476826137713443E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B19" s="5">
+        <f>'MER 7.1'!I81</f>
+        <v>226.114</v>
+      </c>
+      <c r="C19" s="5">
+        <f>'MER 7.1'!B81</f>
+        <v>3877.453</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="2"/>
+        <v>5.8315084670271959E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B20" s="5">
+        <f>'MER 7.1'!I82</f>
+        <v>219.23400000000001</v>
+      </c>
+      <c r="C20" s="5">
+        <f>'MER 7.1'!B82</f>
+        <v>4017.9659999999999</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="2"/>
+        <v>5.456342836151426E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21" s="5">
+        <f>'MER 7.1'!I83</f>
+        <v>261.5</v>
+      </c>
+      <c r="C21" s="5">
+        <f>'MER 7.1'!B83</f>
+        <v>3955.7809999999999</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="2"/>
+        <v>6.6105782903553054E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="11">
+        <f>AVERAGE(D2:D21)</f>
+        <v>6.5086831191752695E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3797,15 +4034,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.3984375" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>2015</v>
@@ -3916,153 +4153,153 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>33</v>
+    <row r="2" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="4">
-        <f>Calculations!D21</f>
-        <v>6.7057173983583865E-2</v>
+        <f>Calculations!D25</f>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="C2" s="4">
         <f>$B2</f>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2:AK2" si="0">$B2</f>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="E2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="F2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="G2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="H2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="I2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="K2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="L2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="M2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="N2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="O2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="P2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="Q2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="R2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="S2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="T2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="U2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="V2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="W2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="X2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="Y2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="Z2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AA2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AB2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AC2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AD2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AE2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AF2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AH2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AI2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AJ2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
       <c r="AK2" s="4">
         <f t="shared" si="0"/>
-        <v>6.7057173983583865E-2</v>
+        <v>6.5086831191752695E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated brpspty and btadlp
</commit_message>
<xml_diff>
--- a/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
+++ b/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\BTaDLP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\us-eps\InputData\elec\BTaDLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F679011A-68B2-4B8A-9BFC-1C6A29282BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="1440" yWindow="1515" windowWidth="15990" windowHeight="14955" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,19 @@
     <sheet name="Calculations" sheetId="4" r:id="rId3"/>
     <sheet name="BTaDLP" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -72,9 +85,6 @@
     <t>Transmission and Distribution Losses and Unaccounted for</t>
   </si>
   <si>
-    <t>Electricity Retail Sales, Total</t>
-  </si>
-  <si>
     <t>Electricity Direct Use</t>
   </si>
   <si>
@@ -85,15 +95,6 @@
   </si>
   <si>
     <t>Net Generation: Electric Power Sector</t>
-  </si>
-  <si>
-    <t>Next Update: October 26, 2016</t>
-  </si>
-  <si>
-    <t>Release Date: September 25, 2016</t>
-  </si>
-  <si>
-    <t>September 2016 Monthly Energy Review</t>
   </si>
   <si>
     <t>No meaningful trend since 2000, so we assume T&amp;D losses going forward are constant at the average value for this period.</t>
@@ -128,11 +129,23 @@
   <si>
     <t>https://www.eia.gov/totalenergy/data/monthly/</t>
   </si>
+  <si>
+    <t>May 2022 Monthly Energy Review</t>
+  </si>
+  <si>
+    <t>Release Date: May 25, 2022</t>
+  </si>
+  <si>
+    <t>Next Update: June 27, 2022</t>
+  </si>
+  <si>
+    <t>Electricity Sales to Ultimate Customers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -225,7 +238,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -234,21 +247,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -344,16 +356,16 @@
                   <c:v>6.2284686986993069E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1476826137713443E-2</c:v>
+                  <c:v>6.1478867955155558E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.8315084670271959E-2</c:v>
+                  <c:v>5.8355059365000683E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.456342836151426E-2</c:v>
+                  <c:v>5.466273552094774E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.6105782903553054E-2</c:v>
+                  <c:v>5.3580150841140213E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,7 +452,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -534,6 +552,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -569,6 +604,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -744,21 +796,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,44 +818,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -811,125 +863,121 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD64"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="9" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="6"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="str">
+    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="str">
         <f>HYPERLINK("http://www.eia.gov/totalenergy/data/monthly/dataunits.cfm","Note: Information about data precision.")</f>
         <v>Note: Information about data precision.</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A9" s="7" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="L11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1949</v>
       </c>
@@ -937,7 +985,7 @@
         <v>291.10000000000002</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>5.0250000000000004</v>
@@ -961,13 +1009,13 @@
         <v>254.511</v>
       </c>
       <c r="K13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L13">
         <v>254.511</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1950</v>
       </c>
@@ -975,7 +1023,7 @@
         <v>329.14100000000002</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>4.9459999999999997</v>
@@ -999,13 +1047,13 @@
         <v>291.44299999999998</v>
       </c>
       <c r="K14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L14">
         <v>291.44299999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1951</v>
       </c>
@@ -1013,7 +1061,7 @@
         <v>370.673</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15">
         <v>4.6260000000000003</v>
@@ -1037,13 +1085,13 @@
         <v>330.28500000000003</v>
       </c>
       <c r="K15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L15">
         <v>330.28500000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1952</v>
       </c>
@@ -1051,7 +1099,7 @@
         <v>399.22399999999999</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16">
         <v>4.6059999999999999</v>
@@ -1075,13 +1123,13 @@
         <v>356.16399999999999</v>
       </c>
       <c r="K16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L16">
         <v>356.16399999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1953</v>
       </c>
@@ -1089,7 +1137,7 @@
         <v>442.66500000000002</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>4.3840000000000003</v>
@@ -1113,13 +1161,13 @@
         <v>396.21699999999998</v>
       </c>
       <c r="K17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17">
         <v>396.21699999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1954</v>
       </c>
@@ -1127,7 +1175,7 @@
         <v>471.68599999999998</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>4.5709999999999997</v>
@@ -1151,13 +1199,13 @@
         <v>424.16399999999999</v>
       </c>
       <c r="K18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L18">
         <v>424.16399999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1955</v>
       </c>
@@ -1165,7 +1213,7 @@
         <v>547.03800000000001</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19">
         <v>3.2610000000000001</v>
@@ -1189,13 +1237,13 @@
         <v>496.74799999999999</v>
       </c>
       <c r="K19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19">
         <v>496.74799999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1956</v>
       </c>
@@ -1203,7 +1251,7 @@
         <v>600.66800000000001</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>3.2080000000000002</v>
@@ -1227,13 +1275,13 @@
         <v>546.28</v>
       </c>
       <c r="K20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L20">
         <v>546.28</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1957</v>
       </c>
@@ -1241,7 +1289,7 @@
         <v>631.51700000000005</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21">
         <v>3.125</v>
@@ -1265,13 +1313,13 @@
         <v>575.82000000000005</v>
       </c>
       <c r="K21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L21">
         <v>575.82000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1958</v>
       </c>
@@ -1279,7 +1327,7 @@
         <v>645.09799999999996</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22">
         <v>3.3519999999999999</v>
@@ -1303,13 +1351,13 @@
         <v>587.86300000000006</v>
       </c>
       <c r="K22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L22">
         <v>587.86300000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1959</v>
       </c>
@@ -1317,7 +1365,7 @@
         <v>710.00599999999997</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23">
         <v>3.3730000000000002</v>
@@ -1341,13 +1389,13 @@
         <v>646.88800000000003</v>
       </c>
       <c r="K23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L23">
         <v>646.88800000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1960</v>
       </c>
@@ -1355,7 +1403,7 @@
         <v>755.54899999999998</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24">
         <v>3.6070000000000002</v>
@@ -1379,13 +1427,13 @@
         <v>688.07500000000005</v>
       </c>
       <c r="K24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L24">
         <v>688.07500000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1961</v>
       </c>
@@ -1393,7 +1441,7 @@
         <v>793.76</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25">
         <v>3.3650000000000002</v>
@@ -1417,13 +1465,13 @@
         <v>721.95</v>
       </c>
       <c r="K25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L25">
         <v>721.95</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1962</v>
       </c>
@@ -1431,7 +1479,7 @@
         <v>854.53499999999997</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26">
         <v>3.4089999999999998</v>
@@ -1455,13 +1503,13 @@
         <v>777.6</v>
       </c>
       <c r="K26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L26">
         <v>777.6</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1963</v>
       </c>
@@ -1469,7 +1517,7 @@
         <v>916.79300000000001</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27">
         <v>3.2349999999999999</v>
@@ -1493,13 +1541,13 @@
         <v>832.61300000000006</v>
       </c>
       <c r="K27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L27">
         <v>832.61300000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1964</v>
       </c>
@@ -1507,7 +1555,7 @@
         <v>983.99</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28">
         <v>3.2280000000000002</v>
@@ -1531,13 +1579,13 @@
         <v>896.05899999999997</v>
       </c>
       <c r="K28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L28">
         <v>896.05899999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1965</v>
       </c>
@@ -1545,7 +1593,7 @@
         <v>1055.252</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29">
         <v>3.1339999999999999</v>
@@ -1569,13 +1617,13 @@
         <v>953.78899999999999</v>
       </c>
       <c r="K29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L29">
         <v>953.78899999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1966</v>
       </c>
@@ -1583,7 +1631,7 @@
         <v>1144.3499999999999</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30">
         <v>3.1819999999999999</v>
@@ -1607,13 +1655,13 @@
         <v>1035.145</v>
       </c>
       <c r="K30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L30">
         <v>1035.145</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1967</v>
       </c>
@@ -1621,7 +1669,7 @@
         <v>1214.365</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31">
         <v>3.431</v>
@@ -1645,13 +1693,13 @@
         <v>1099.2170000000001</v>
       </c>
       <c r="K31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L31">
         <v>1099.2170000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1968</v>
       </c>
@@ -1659,7 +1707,7 @@
         <v>1329.443</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32">
         <v>3.383</v>
@@ -1683,13 +1731,13 @@
         <v>1202.8710000000001</v>
       </c>
       <c r="K32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L32">
         <v>1202.8710000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1969</v>
       </c>
@@ -1697,7 +1745,7 @@
         <v>1442.182</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D33">
         <v>3.2759999999999998</v>
@@ -1721,13 +1769,13 @@
         <v>1313.8330000000001</v>
       </c>
       <c r="K33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L33">
         <v>1313.8330000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1970</v>
       </c>
@@ -1735,7 +1783,7 @@
         <v>1531.8679999999999</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34">
         <v>3.2440000000000002</v>
@@ -1759,13 +1807,13 @@
         <v>1392.3</v>
       </c>
       <c r="K34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L34">
         <v>1392.3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1971</v>
       </c>
@@ -1773,7 +1821,7 @@
         <v>1612.633</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35">
         <v>3.2210000000000001</v>
@@ -1797,13 +1845,13 @@
         <v>1469.54</v>
       </c>
       <c r="K35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L35">
         <v>1469.54</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1972</v>
       </c>
@@ -1811,7 +1859,7 @@
         <v>1749.662</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D36">
         <v>3.3159999999999998</v>
@@ -1835,13 +1883,13 @@
         <v>1595.1610000000001</v>
       </c>
       <c r="K36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L36">
         <v>1595.1610000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1973</v>
       </c>
@@ -1849,7 +1897,7 @@
         <v>1860.71</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37">
         <v>3.347</v>
@@ -1873,13 +1921,13 @@
         <v>1712.9090000000001</v>
       </c>
       <c r="K37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L37">
         <v>1712.9090000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>1974</v>
       </c>
@@ -1887,7 +1935,7 @@
         <v>1867.14</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38">
         <v>3.18</v>
@@ -1911,13 +1959,13 @@
         <v>1705.924</v>
       </c>
       <c r="K38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L38">
         <v>1705.924</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>1975</v>
       </c>
@@ -1925,7 +1973,7 @@
         <v>1917.6489999999999</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39">
         <v>3.1059999999999999</v>
@@ -1949,13 +1997,13 @@
         <v>1747.0909999999999</v>
       </c>
       <c r="K39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L39">
         <v>1747.0909999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>1976</v>
       </c>
@@ -1963,7 +2011,7 @@
         <v>2037.6959999999999</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40">
         <v>3.2170000000000001</v>
@@ -1987,13 +2035,13 @@
         <v>1855.2460000000001</v>
       </c>
       <c r="K40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L40">
         <v>1855.2460000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>1977</v>
       </c>
@@ -2001,7 +2049,7 @@
         <v>2124.3229999999999</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>3.1240000000000001</v>
@@ -2025,13 +2073,13 @@
         <v>1948.3610000000001</v>
       </c>
       <c r="K41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L41">
         <v>1948.3610000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>1978</v>
       </c>
@@ -2039,7 +2087,7 @@
         <v>2206.3310000000001</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42">
         <v>3.0459999999999998</v>
@@ -2063,13 +2111,13 @@
         <v>2017.922</v>
       </c>
       <c r="K42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L42">
         <v>2017.922</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>1979</v>
       </c>
@@ -2077,7 +2125,7 @@
         <v>2247.3719999999998</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D43">
         <v>3.2930000000000001</v>
@@ -2101,13 +2149,13 @@
         <v>2071.0990000000002</v>
       </c>
       <c r="K43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L43">
         <v>2071.0990000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>1980</v>
       </c>
@@ -2115,7 +2163,7 @@
         <v>2286.4389999999999</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44">
         <v>3.161</v>
@@ -2139,13 +2187,13 @@
         <v>2094.4490000000001</v>
       </c>
       <c r="K44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L44">
         <v>2094.4490000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>1981</v>
       </c>
@@ -2153,7 +2201,7 @@
         <v>2294.8119999999999</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45">
         <v>3.161</v>
@@ -2177,13 +2225,13 @@
         <v>2147.1030000000001</v>
       </c>
       <c r="K45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L45">
         <v>2147.1030000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>1982</v>
       </c>
@@ -2191,7 +2239,7 @@
         <v>2241.2109999999998</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D46">
         <v>3.161</v>
@@ -2215,13 +2263,13 @@
         <v>2086.4409999999998</v>
       </c>
       <c r="K46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L46">
         <v>2086.4409999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1983</v>
       </c>
@@ -2229,7 +2277,7 @@
         <v>2310.2849999999999</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D47">
         <v>3.161</v>
@@ -2253,13 +2301,13 @@
         <v>2150.9549999999999</v>
       </c>
       <c r="K47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L47">
         <v>2150.9549999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>1984</v>
       </c>
@@ -2267,7 +2315,7 @@
         <v>2416.3040000000001</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D48">
         <v>3.161</v>
@@ -2291,13 +2339,13 @@
         <v>2285.7959999999998</v>
       </c>
       <c r="K48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L48">
         <v>2285.7959999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1985</v>
       </c>
@@ -2305,7 +2353,7 @@
         <v>2469.8409999999999</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D49">
         <v>3.161</v>
@@ -2329,13 +2377,13 @@
         <v>2323.9740000000002</v>
       </c>
       <c r="K49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L49">
         <v>2323.9740000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>1986</v>
       </c>
@@ -2343,7 +2391,7 @@
         <v>2487.31</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D50">
         <v>3.161</v>
@@ -2367,13 +2415,13 @@
         <v>2368.7530000000002</v>
       </c>
       <c r="K50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L50">
         <v>2368.7530000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1987</v>
       </c>
@@ -2381,7 +2429,7 @@
         <v>2572.127</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51">
         <v>3.161</v>
@@ -2405,13 +2453,13 @@
         <v>2457.2719999999999</v>
       </c>
       <c r="K51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L51">
         <v>2457.2719999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>1988</v>
       </c>
@@ -2419,7 +2467,7 @@
         <v>2704.25</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D52">
         <v>3.161</v>
@@ -2443,13 +2491,13 @@
         <v>2578.0619999999999</v>
       </c>
       <c r="K52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L52">
         <v>2578.0619999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>1989</v>
       </c>
@@ -2487,7 +2535,7 @@
         <v>2755.6350000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>1990</v>
       </c>
@@ -2525,7 +2573,7 @@
         <v>2837.0839999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>1991</v>
       </c>
@@ -2563,7 +2611,7 @@
         <v>2886.06</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>1992</v>
       </c>
@@ -2601,7 +2649,7 @@
         <v>2897.2069999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1993</v>
       </c>
@@ -2639,7 +2687,7 @@
         <v>3000.7</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>1994</v>
       </c>
@@ -2677,7 +2725,7 @@
         <v>3080.8879999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>1995</v>
       </c>
@@ -2715,7 +2763,7 @@
         <v>3163.9630000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>1996</v>
       </c>
@@ -2753,7 +2801,7 @@
         <v>3253.7649999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>1997</v>
       </c>
@@ -2791,7 +2839,7 @@
         <v>3301.8490000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>1998</v>
       </c>
@@ -2829,7 +2877,7 @@
         <v>3425.0970000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>1999</v>
       </c>
@@ -2867,7 +2915,7 @@
         <v>3483.7159999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>2000</v>
       </c>
@@ -2905,7 +2953,7 @@
         <v>3592.357</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>2001</v>
       </c>
@@ -2943,7 +2991,7 @@
         <v>3557.107</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>2002</v>
       </c>
@@ -2981,7 +3029,7 @@
         <v>3631.65</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>2003</v>
       </c>
@@ -3019,7 +3067,7 @@
         <v>3662.029</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>2004</v>
       </c>
@@ -3057,7 +3105,7 @@
         <v>3715.9490000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>2005</v>
       </c>
@@ -3095,7 +3143,7 @@
         <v>3810.9839999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>2006</v>
       </c>
@@ -3133,7 +3181,7 @@
         <v>3816.8449999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>2007</v>
       </c>
@@ -3171,7 +3219,7 @@
         <v>3890.2310000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>2008</v>
       </c>
@@ -3209,7 +3257,7 @@
         <v>3866.1610000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>2009</v>
       </c>
@@ -3247,7 +3295,7 @@
         <v>3723.7330000000002</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>2010</v>
       </c>
@@ -3285,7 +3333,7 @@
         <v>3886.752</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>2011</v>
       </c>
@@ -3323,7 +3371,7 @@
         <v>3882.6</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>2012</v>
       </c>
@@ -3361,7 +3409,7 @@
         <v>3832.306</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>2013</v>
       </c>
@@ -3399,7 +3447,7 @@
         <v>3868.33</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>2014</v>
       </c>
@@ -3437,7 +3485,7 @@
         <v>3903.2739999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>2015</v>
       </c>
@@ -3475,7 +3523,7 @@
         <v>3900.16</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>2016</v>
       </c>
@@ -3501,19 +3549,19 @@
         <v>66.501999999999995</v>
       </c>
       <c r="I80">
-        <v>240.87100000000001</v>
+        <v>240.87899999999999</v>
       </c>
       <c r="J80">
         <v>3762.462</v>
       </c>
       <c r="K80">
-        <v>139.84399999999999</v>
+        <v>139.83699999999999</v>
       </c>
       <c r="L80">
-        <v>3902.306</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+        <v>3902.2979999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>2017</v>
       </c>
@@ -3539,24 +3587,24 @@
         <v>56.314</v>
       </c>
       <c r="I81">
-        <v>226.114</v>
+        <v>226.26900000000001</v>
       </c>
       <c r="J81">
         <v>3723.3560000000002</v>
       </c>
       <c r="K81">
-        <v>141.114</v>
+        <v>140.959</v>
       </c>
       <c r="L81">
-        <v>3864.47</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+        <v>3864.3150000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>2018</v>
       </c>
       <c r="B82">
-        <v>4017.9659999999999</v>
+        <v>4018.1669999999999</v>
       </c>
       <c r="C82">
         <v>13.311999999999999</v>
@@ -3565,7 +3613,7 @@
         <v>146.798</v>
       </c>
       <c r="E82">
-        <v>4178.0770000000002</v>
+        <v>4178.277</v>
       </c>
       <c r="F82">
         <v>58.261000000000003</v>
@@ -3577,33 +3625,33 @@
         <v>44.456000000000003</v>
       </c>
       <c r="I82">
-        <v>219.23400000000001</v>
+        <v>219.64400000000001</v>
       </c>
       <c r="J82">
         <v>3859.1849999999999</v>
       </c>
       <c r="K82">
-        <v>144.114</v>
+        <v>143.904</v>
       </c>
       <c r="L82">
-        <v>4003.299</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+        <v>4003.0889999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>2019</v>
       </c>
       <c r="B83">
-        <v>3955.7809999999999</v>
+        <v>3965.6289999999999</v>
       </c>
       <c r="C83">
-        <v>13.624000000000001</v>
+        <v>13.689</v>
       </c>
       <c r="D83">
-        <v>148.64500000000001</v>
+        <v>148.53700000000001</v>
       </c>
       <c r="E83">
-        <v>4118.0510000000004</v>
+        <v>4127.8549999999996</v>
       </c>
       <c r="F83">
         <v>59.052</v>
@@ -3615,52 +3663,131 @@
         <v>39.043999999999997</v>
       </c>
       <c r="I83">
-        <v>261.5</v>
+        <v>212.47900000000001</v>
       </c>
       <c r="J83">
-        <v>3749.538</v>
+        <v>3811.15</v>
       </c>
       <c r="K83">
-        <v>146.05699999999999</v>
+        <v>143.27000000000001</v>
       </c>
       <c r="L83">
-        <v>3895.5949999999998</v>
+        <v>3954.4209999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B84">
+        <v>3851.0340000000001</v>
+      </c>
+      <c r="C84">
+        <v>13.045999999999999</v>
+      </c>
+      <c r="D84">
+        <v>143.05600000000001</v>
+      </c>
+      <c r="E84">
+        <v>4007.1350000000002</v>
+      </c>
+      <c r="F84">
+        <v>61.448999999999998</v>
+      </c>
+      <c r="G84">
+        <v>14.135</v>
+      </c>
+      <c r="H84">
+        <v>47.314</v>
+      </c>
+      <c r="I84">
+        <v>198.08500000000001</v>
+      </c>
+      <c r="J84">
+        <v>3717.674</v>
+      </c>
+      <c r="K84">
+        <v>138.69</v>
+      </c>
+      <c r="L84">
+        <v>3856.364</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B85">
+        <v>3962.7849999999999</v>
+      </c>
+      <c r="C85">
+        <v>13.148</v>
+      </c>
+      <c r="D85">
+        <v>139.607</v>
+      </c>
+      <c r="E85">
+        <v>4115.54</v>
+      </c>
+      <c r="F85">
+        <v>53.167000000000002</v>
+      </c>
+      <c r="G85">
+        <v>13.840999999999999</v>
+      </c>
+      <c r="H85">
+        <v>39.325000000000003</v>
+      </c>
+      <c r="I85">
+        <v>224.61</v>
+      </c>
+      <c r="J85">
+        <v>3794.5390000000002</v>
+      </c>
+      <c r="K85">
+        <v>135.71600000000001</v>
+      </c>
+      <c r="L85">
+        <v>3930.2550000000001</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="http://www.eia.gov/totalenergy/data/monthly/dataunits.cfm" xr:uid="{1F9F0B60-66F6-4414-A588-5F90C9C12287}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.265625" customWidth="1"/>
-    <col min="4" max="4" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2000</v>
       </c>
@@ -3677,7 +3804,7 @@
         <v>6.6944071098814603E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2001</v>
       </c>
@@ -3694,7 +3821,7 @@
         <v>5.6301959775455837E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2002</v>
       </c>
@@ -3711,7 +3838,7 @@
         <v>6.69968403047973E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2003</v>
       </c>
@@ -3728,7 +3855,7 @@
         <v>6.1157289973365822E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2004</v>
       </c>
@@ -3745,7 +3872,7 @@
         <v>6.9824806478379145E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2005</v>
       </c>
@@ -3762,7 +3889,7 @@
         <v>6.8991223394440859E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2006</v>
       </c>
@@ -3779,7 +3906,7 @@
         <v>6.8135044422103247E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2007</v>
       </c>
@@ -3796,7 +3923,7 @@
         <v>7.4342197409809851E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2008</v>
       </c>
@@ -3813,7 +3940,7 @@
         <v>7.1973548372324628E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2009</v>
       </c>
@@ -3830,7 +3957,7 @@
         <v>6.8415000431776993E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2010</v>
       </c>
@@ -3847,7 +3974,7 @@
         <v>6.6530543607796436E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2011</v>
       </c>
@@ -3864,7 +3991,7 @@
         <v>6.4533940396931652E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2012</v>
       </c>
@@ -3881,7 +4008,7 @@
         <v>6.7531060123515632E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2013</v>
       </c>
@@ -3898,7 +4025,7 @@
         <v>6.5453036402503759E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2014</v>
       </c>
@@ -3915,7 +4042,7 @@
         <v>6.18602525829927E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2015</v>
       </c>
@@ -3932,13 +4059,13 @@
         <v>6.2284686986993069E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2016</v>
       </c>
       <c r="B18" s="5">
         <f>'MER 7.1'!I80</f>
-        <v>240.87100000000001</v>
+        <v>240.87899999999999</v>
       </c>
       <c r="C18" s="5">
         <f>'MER 7.1'!B80</f>
@@ -3946,16 +4073,16 @@
       </c>
       <c r="D18" s="4">
         <f t="shared" ref="D18:D21" si="2">B18/C18</f>
-        <v>6.1476826137713443E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+        <v>6.1478867955155558E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2017</v>
       </c>
       <c r="B19" s="5">
         <f>'MER 7.1'!I81</f>
-        <v>226.114</v>
+        <v>226.26900000000001</v>
       </c>
       <c r="C19" s="5">
         <f>'MER 7.1'!B81</f>
@@ -3963,57 +4090,97 @@
       </c>
       <c r="D19" s="4">
         <f t="shared" si="2"/>
-        <v>5.8315084670271959E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5.8355059365000683E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2018</v>
       </c>
       <c r="B20" s="5">
         <f>'MER 7.1'!I82</f>
-        <v>219.23400000000001</v>
+        <v>219.64400000000001</v>
       </c>
       <c r="C20" s="5">
         <f>'MER 7.1'!B82</f>
-        <v>4017.9659999999999</v>
+        <v>4018.1669999999999</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="2"/>
-        <v>5.456342836151426E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5.466273552094774E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2019</v>
       </c>
       <c r="B21" s="5">
         <f>'MER 7.1'!I83</f>
-        <v>261.5</v>
+        <v>212.47900000000001</v>
       </c>
       <c r="C21" s="5">
         <f>'MER 7.1'!B83</f>
-        <v>3955.7809999999999</v>
+        <v>3965.6289999999999</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="2"/>
-        <v>6.6105782903553054E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="11">
-        <f>AVERAGE(D2:D21)</f>
-        <v>6.5086831191752695E-2</v>
+        <v>5.3580150841140213E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B22" s="5">
+        <f>'MER 7.1'!I84</f>
+        <v>198.08500000000001</v>
+      </c>
+      <c r="C22" s="5">
+        <f>'MER 7.1'!B84</f>
+        <v>3851.0340000000001</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" ref="D22:D23" si="3">B22/C22</f>
+        <v>5.1436834886422714E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B23" s="5">
+        <f>'MER 7.1'!I85</f>
+        <v>224.61</v>
+      </c>
+      <c r="C23" s="5">
+        <f>'MER 7.1'!B85</f>
+        <v>3962.7849999999999</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="3"/>
+        <v>5.667983501502101E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="6">
+        <f>AVERAGE(D2:D23)</f>
+        <v>6.3521317515713147E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4024,25 +4191,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.3984375" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1">
         <v>2015</v>
@@ -4153,153 +4320,153 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
-        <v>31</v>
+    <row r="2" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="4">
-        <f>Calculations!D25</f>
-        <v>6.5086831191752695E-2</v>
+        <f>Calculations!D28</f>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="C2" s="4">
         <f>$B2</f>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2:AK2" si="0">$B2</f>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="E2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="F2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="G2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="H2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="I2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="K2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="L2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="M2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="N2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="O2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="P2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="Q2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="R2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="S2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="T2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="U2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="V2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="W2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="X2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="Y2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="Z2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AA2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AB2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AC2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AD2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AE2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AF2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AH2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AI2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AJ2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
       <c r="AK2" s="4">
         <f t="shared" si="0"/>
-        <v>6.5086831191752695E-2</v>
+        <v>6.3521317515713147E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>